<commit_message>
added params to uncaging stuff
</commit_message>
<xml_diff>
--- a/result_table_templates/Uncaging.xlsx
+++ b/result_table_templates/Uncaging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregschwartz/matlab/DJ_schwartzlab/result_table_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C88AC1D-0639-9B42-99F1-1057D9A699CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F10FB5-B64E-F04E-A205-6D9329BC7384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="960" windowWidth="30860" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="960" windowWidth="26020" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Field</t>
   </si>
@@ -89,6 +89,48 @@
   </si>
   <si>
     <t>time axis for each trace</t>
+  </si>
+  <si>
+    <t>laser_power</t>
+  </si>
+  <si>
+    <t>laser power (percent)</t>
+  </si>
+  <si>
+    <t>laser_wavelength</t>
+  </si>
+  <si>
+    <t>laser wavelength</t>
+  </si>
+  <si>
+    <t>shutter_open</t>
+  </si>
+  <si>
+    <t>T or F for shutter open</t>
+  </si>
+  <si>
+    <t>drug_condition</t>
+  </si>
+  <si>
+    <t>drugs in the bath (free text)</t>
+  </si>
+  <si>
+    <t>number_of_sequences</t>
+  </si>
+  <si>
+    <t>number_of_stim_groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of repeats </t>
+  </si>
+  <si>
+    <t>number of different uncaging locations</t>
+  </si>
+  <si>
+    <t>group_names</t>
+  </si>
+  <si>
+    <t>free text used to associate ROI files with this epoch</t>
   </si>
 </sst>
 </file>
@@ -147,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="297" zoomScaleNormal="297" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="297" zoomScaleNormal="297" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -555,6 +597,83 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>